<commit_message>
minor wording changes for 7/5-7/7, also preview of 7/8
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-07-07.xlsx
+++ b/EC/Train Runs and Enforcements 2016-07-07.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Train Runs" sheetId="1" r:id="rId1"/>
@@ -2941,525 +2941,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_XINGS" xfId="1"/>
   </cellStyles>
-  <dxfs count="89">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -3556,30 +3038,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3886,7 +3344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM208"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4538,12 +3996,12 @@
         <v>0101-07</v>
       </c>
       <c r="AE13" s="108" t="str">
-        <f t="shared" ref="AE13:AE44" si="0">"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B13&amp;"/"&amp;TEXT(F13,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13,"YYYY-MM-DD")
+        <f t="shared" ref="AE13:AE14" si="0">"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B13&amp;"/"&amp;TEXT(F13,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13,"YYYY-MM-DD")
 &amp;" &amp; "&amp;"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B13&amp;"/"&amp;TEXT(F13+1,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13+1,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B13&amp;"\"&amp;TEXT(F13+1,"YYYY-MM-DD")</f>
         <v>aws s3 cp s3://rtdc.mdm.uploadarchive/RTDC4007/2016-07-07/ "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4007\2016-07-07 --recursive &amp; "C:\Users\stu\Documents\GitHub\mrs-test-scripts\Headless Mode &amp; Sideloading\WalkAndUnGZ.bat" "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4007\2016-07-07 &amp; aws s3 cp s3://rtdc.mdm.uploadarchive/RTDC4007/2016-07-08/ "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4007\2016-07-08 --recursive &amp; "C:\Users\stu\Documents\GitHub\mrs-test-scripts\Headless Mode &amp; Sideloading\WalkAndUnGZ.bat" "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4007\2016-07-08</v>
       </c>
       <c r="AF13" s="108" t="str">
-        <f t="shared" ref="AF13:AF44" si="1">astrogrep_path&amp;" /spath="&amp;search_path&amp;" /stypes=""*"&amp;B13&amp;"*"&amp;TEXT(F13-utc_offset/24,"YYYYMMDD")&amp;"*"" /stext="" "&amp;TEXT(F13-utc_offset/24,"HH")&amp;search_regexp&amp;""" /e /r /s"</f>
+        <f t="shared" ref="AF13:AF14" si="1">astrogrep_path&amp;" /spath="&amp;search_path&amp;" /stypes=""*"&amp;B13&amp;"*"&amp;TEXT(F13-utc_offset/24,"YYYYMMDD")&amp;"*"" /stext="" "&amp;TEXT(F13-utc_offset/24,"HH")&amp;search_regexp&amp;""" /e /r /s"</f>
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4007*20160707*" /stext=" 09:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
     </row>
@@ -4814,7 +4272,7 @@
         <v>734</v>
       </c>
       <c r="S16" s="54">
-        <f t="shared" ref="S15:S78" si="14">SUM(U16:U16)/12</f>
+        <f t="shared" ref="S16:S78" si="14">SUM(U16:U16)/12</f>
         <v>1</v>
       </c>
       <c r="T16" s="98" t="str">
@@ -5019,7 +4477,7 @@
         <v>2.7141203703649808E-2</v>
       </c>
       <c r="N18" s="7">
-        <f t="shared" ref="N15:P78" si="15">24*60*SUM($M18:$M18)</f>
+        <f t="shared" ref="N18:P78" si="15">24*60*SUM($M18:$M18)</f>
         <v>39.083333333255723</v>
       </c>
       <c r="O18" s="7"/>
@@ -20140,7 +19598,7 @@
         <v>0</v>
       </c>
       <c r="K158" s="34" t="str">
-        <f t="shared" ref="K154:K158" si="44">IF(ISEVEN(B158),(B158-1)&amp;"/"&amp;B158,B158&amp;"/"&amp;(B158+1))</f>
+        <f t="shared" ref="K158" si="44">IF(ISEVEN(B158),(B158-1)&amp;"/"&amp;B158,B158&amp;"/"&amp;(B158+1))</f>
         <v>4025/4026</v>
       </c>
       <c r="L158" s="34" t="str">
@@ -20148,7 +19606,7 @@
         <v>BEAM</v>
       </c>
       <c r="M158" s="6">
-        <f t="shared" ref="M154:M158" si="45">I158-F158</f>
+        <f t="shared" ref="M158" si="45">I158-F158</f>
         <v>8.5300925929914229E-3</v>
       </c>
       <c r="N158" s="7"/>
@@ -20175,12 +19633,12 @@
         <v>0800-07</v>
       </c>
       <c r="AE158" s="108" t="str">
-        <f t="shared" ref="AE141:AE172" si="48">"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B158&amp;"/"&amp;TEXT(F158,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158,"YYYY-MM-DD")
+        <f t="shared" ref="AE158:AE172" si="48">"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B158&amp;"/"&amp;TEXT(F158,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158,"YYYY-MM-DD")
 &amp;" &amp; "&amp;"aws s3 cp "&amp;s3_bucket&amp;"/RTDC"&amp;B158&amp;"/"&amp;TEXT(F158+1,"YYYY-MM-DD")&amp;"/ "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158+1,"YYYY-MM-DD")&amp;" --recursive &amp; """&amp;walkandungz&amp;""" "&amp;search_path&amp;"\RTDC"&amp;B158&amp;"\"&amp;TEXT(F158+1,"YYYY-MM-DD")</f>
         <v>aws s3 cp s3://rtdc.mdm.uploadarchive/RTDC4026/2016-07-07/ "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4026\2016-07-07 --recursive &amp; "C:\Users\stu\Documents\GitHub\mrs-test-scripts\Headless Mode &amp; Sideloading\WalkAndUnGZ.bat" "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4026\2016-07-07 &amp; aws s3 cp s3://rtdc.mdm.uploadarchive/RTDC4026/2016-07-08/ "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4026\2016-07-08 --recursive &amp; "C:\Users\stu\Documents\GitHub\mrs-test-scripts\Headless Mode &amp; Sideloading\WalkAndUnGZ.bat" "C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations"\RTDC4026\2016-07-08</v>
       </c>
       <c r="AF158" s="108" t="str">
-        <f t="shared" ref="AF141:AF172" si="49">astrogrep_path&amp;" /spath="&amp;search_path&amp;" /stypes=""*"&amp;B158&amp;"*"&amp;TEXT(F158-utc_offset/24,"YYYYMMDD")&amp;"*"" /stext="" "&amp;TEXT(F158-utc_offset/24,"HH")&amp;search_regexp&amp;""" /e /r /s"</f>
+        <f t="shared" ref="AF158:AF172" si="49">astrogrep_path&amp;" /spath="&amp;search_path&amp;" /stypes=""*"&amp;B158&amp;"*"&amp;TEXT(F158-utc_offset/24,"YYYYMMDD")&amp;"*"" /stext="" "&amp;TEXT(F158-utc_offset/24,"HH")&amp;search_regexp&amp;""" /e /r /s"</f>
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4026*20160707*" /stext=" 11:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
     </row>
@@ -23948,37 +23406,37 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="W11:W12 W13:X1048576">
-    <cfRule type="cellIs" dxfId="85" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="75" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X1048576">
-    <cfRule type="cellIs" dxfId="84" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="58" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X1048576">
-    <cfRule type="cellIs" dxfId="83" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:J13 L13:S13 A15:J139 A141:J156 A14:S14 K15:S208">
-    <cfRule type="expression" dxfId="82" priority="51">
+    <cfRule type="expression" dxfId="8" priority="51">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:J13 L13:S13 A15:J139 A141:J156 A14:S14 K15:S208">
-    <cfRule type="expression" dxfId="81" priority="50">
+    <cfRule type="expression" dxfId="7" priority="50">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="80" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="79" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24023,7 +23481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T120"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24226,11 +23686,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4011*20160707*" /stext=" 12:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S7" s="10" t="str">
-        <f>MID(B7,13,4)</f>
+        <f t="shared" ref="S7:S38" si="0">MID(B7,13,4)</f>
         <v>4011</v>
       </c>
       <c r="T7" s="61">
-        <f>A7+6/24</f>
+        <f t="shared" ref="T7:T38" si="1">A7+6/24</f>
         <v>42558.538287037038</v>
       </c>
     </row>
@@ -24291,11 +23751,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4031*20160707*" /stext=" 23:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S8" s="10" t="str">
-        <f>MID(B8,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4031</v>
       </c>
       <c r="T8" s="61">
-        <f>A8+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.99728009259</v>
       </c>
     </row>
@@ -24357,11 +23817,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S9" s="10" t="str">
-        <f>MID(B9,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T9" s="61">
-        <f>A9+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.629710648151</v>
       </c>
     </row>
@@ -24423,11 +23883,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S10" s="10" t="str">
-        <f>MID(B10,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T10" s="61">
-        <f>A10+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.946585648147</v>
       </c>
     </row>
@@ -24488,11 +23948,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4044*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S11" s="10" t="str">
-        <f>MID(B11,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4044</v>
       </c>
       <c r="T11" s="61">
-        <f>A11+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.914502314816</v>
       </c>
     </row>
@@ -24553,11 +24013,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4013*20160707*" /stext=" 20:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S12" s="10" t="str">
-        <f>MID(B12,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4013</v>
       </c>
       <c r="T12" s="61">
-        <f>A12+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.881111111114</v>
       </c>
     </row>
@@ -24616,11 +24076,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 03:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S13" s="10" t="str">
-        <f>MID(B13,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T13" s="61">
-        <f>A13+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.141064814816</v>
       </c>
     </row>
@@ -24679,11 +24139,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S14" s="10" t="str">
-        <f>MID(B14,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4025</v>
       </c>
       <c r="T14" s="61">
-        <f>A14+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.606296296297</v>
       </c>
     </row>
@@ -24742,11 +24202,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 10:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S15" s="10" t="str">
-        <f>MID(B15,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4043</v>
       </c>
       <c r="T15" s="61">
-        <f>A15+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.452002314814</v>
       </c>
     </row>
@@ -24805,11 +24265,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4008*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S16" s="10" t="str">
-        <f>MID(B16,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4008</v>
       </c>
       <c r="T16" s="61">
-        <f>A16+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.81459490741</v>
       </c>
     </row>
@@ -24869,11 +24329,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 22:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S17" s="10" t="str">
-        <f>MID(B17,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4043</v>
       </c>
       <c r="T17" s="61">
-        <f>A17+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.969513888886</v>
       </c>
     </row>
@@ -24933,11 +24393,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S18" s="10" t="str">
-        <f>MID(B18,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T18" s="61">
-        <f>A18+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.05841435185</v>
       </c>
     </row>
@@ -24997,11 +24457,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S19" s="10" t="str">
-        <f>MID(B19,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
       <c r="T19" s="61">
-        <f>A19+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.911817129629</v>
       </c>
     </row>
@@ -25061,11 +24521,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S20" s="10" t="str">
-        <f>MID(B20,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
       <c r="T20" s="61">
-        <f>A20+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.911099537036</v>
       </c>
     </row>
@@ -25124,11 +24584,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4028*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S21" s="10" t="str">
-        <f>MID(B21,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4028</v>
       </c>
       <c r="T21" s="61">
-        <f>A21+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.623993055553</v>
       </c>
     </row>
@@ -25187,11 +24647,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 23:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S22" s="10" t="str">
-        <f>MID(B22,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4012</v>
       </c>
       <c r="T22" s="61">
-        <f>A22+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.02065972222</v>
       </c>
     </row>
@@ -25250,11 +24710,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S23" s="10" t="str">
-        <f>MID(B23,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T23" s="61">
-        <f>A23+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.072233796294</v>
       </c>
     </row>
@@ -25313,11 +24773,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S24" s="10" t="str">
-        <f>MID(B24,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T24" s="61">
-        <f>A24+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.894421296296</v>
       </c>
     </row>
@@ -25376,11 +24836,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S25" s="10" t="str">
-        <f>MID(B25,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T25" s="61">
-        <f>A25+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.601956018516</v>
       </c>
     </row>
@@ -25439,11 +24899,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 10:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S26" s="10" t="str">
-        <f>MID(B26,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4043</v>
       </c>
       <c r="T26" s="61">
-        <f>A26+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.448703703703</v>
       </c>
     </row>
@@ -25502,11 +24962,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 23:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S27" s="10" t="str">
-        <f>MID(B27,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4012</v>
       </c>
       <c r="T27" s="61">
-        <f>A27+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.018703703703</v>
       </c>
     </row>
@@ -25566,11 +25026,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S28" s="10" t="str">
-        <f>MID(B28,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T28" s="61">
-        <f>A28+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.632407407407</v>
       </c>
     </row>
@@ -25630,11 +25090,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 00:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S29" s="10" t="str">
-        <f>MID(B29,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T29" s="61">
-        <f>A29+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.018969907411</v>
       </c>
     </row>
@@ -25694,11 +25154,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S30" s="10" t="str">
-        <f>MID(B30,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
       <c r="T30" s="61">
-        <f>A30+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.899687500001</v>
       </c>
     </row>
@@ -25758,11 +25218,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 10:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S31" s="10" t="str">
-        <f>MID(B31,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4025</v>
       </c>
       <c r="T31" s="61">
-        <f>A31+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.456817129627</v>
       </c>
     </row>
@@ -25822,11 +25282,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4026*20160707*" /stext=" 12:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S32" s="10" t="str">
-        <f>MID(B32,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4026</v>
       </c>
       <c r="T32" s="61">
-        <f>A32+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.509421296294</v>
       </c>
     </row>
@@ -25886,11 +25346,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S33" s="10" t="str">
-        <f>MID(B33,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
       <c r="T33" s="61">
-        <f>A33+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.905462962961</v>
       </c>
     </row>
@@ -25950,11 +25410,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160708*" /stext=" 00:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S34" s="10" t="str">
-        <f>MID(B34,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
       <c r="T34" s="61">
-        <f>A34+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.030219907407</v>
       </c>
     </row>
@@ -26014,11 +25474,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4028*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S35" s="10" t="str">
-        <f>MID(B35,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4028</v>
       </c>
       <c r="T35" s="61">
-        <f>A35+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.905428240738</v>
       </c>
     </row>
@@ -26078,11 +25538,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S36" s="10" t="str">
-        <f>MID(B36,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T36" s="61">
-        <f>A36+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.060636574075</v>
       </c>
     </row>
@@ -26142,11 +25602,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S37" s="10" t="str">
-        <f>MID(B37,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4037</v>
       </c>
       <c r="T37" s="61">
-        <f>A37+6/24</f>
+        <f t="shared" si="1"/>
         <v>42559.054548611108</v>
       </c>
     </row>
@@ -26206,11 +25666,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4031*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S38" s="10" t="str">
-        <f>MID(B38,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4031</v>
       </c>
       <c r="T38" s="61">
-        <f>A38+6/24</f>
+        <f t="shared" si="1"/>
         <v>42558.648506944446</v>
       </c>
     </row>
@@ -26270,11 +25730,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4027*20160707*" /stext=" 16:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S39" s="10" t="str">
-        <f>MID(B39,13,4)</f>
+        <f t="shared" ref="S39:S70" si="2">MID(B39,13,4)</f>
         <v>4027</v>
       </c>
       <c r="T39" s="61">
-        <f>A39+6/24</f>
+        <f t="shared" ref="T39:T70" si="3">A39+6/24</f>
         <v>42558.732256944444</v>
       </c>
     </row>
@@ -26336,11 +25796,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4031*20160707*" /stext=" 09:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S40" s="10" t="str">
-        <f>MID(B40,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4031</v>
       </c>
       <c r="T40" s="61">
-        <f>A40+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.411469907405</v>
       </c>
     </row>
@@ -26402,11 +25862,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S41" s="10" t="str">
-        <f>MID(B41,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4040</v>
       </c>
       <c r="T41" s="61">
-        <f>A41+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.601203703707</v>
       </c>
     </row>
@@ -26468,11 +25928,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S42" s="10" t="str">
-        <f>MID(B42,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4025</v>
       </c>
       <c r="T42" s="61">
-        <f>A42+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.581631944442</v>
       </c>
     </row>
@@ -26532,11 +25992,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S43" s="10" t="str">
-        <f>MID(B43,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4039</v>
       </c>
       <c r="T43" s="61">
-        <f>A43+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.738171296296</v>
       </c>
     </row>
@@ -26596,11 +26056,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S44" s="10" t="str">
-        <f>MID(B44,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4039</v>
       </c>
       <c r="T44" s="61">
-        <f>A44+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.738854166666</v>
       </c>
     </row>
@@ -26660,11 +26120,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4039*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S45" s="10" t="str">
-        <f>MID(B45,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4039</v>
       </c>
       <c r="T45" s="61">
-        <f>A45+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.739548611113</v>
       </c>
     </row>
@@ -26726,11 +26186,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4027*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S46" s="10" t="str">
-        <f>MID(B46,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4027</v>
       </c>
       <c r="T46" s="61">
-        <f>A46+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.568831018521</v>
       </c>
     </row>
@@ -26792,11 +26252,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S47" s="10" t="str">
-        <f>MID(B47,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4037</v>
       </c>
       <c r="T47" s="61">
-        <f>A47+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.948796296296</v>
       </c>
     </row>
@@ -26858,11 +26318,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4044*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S48" s="10" t="str">
-        <f>MID(B48,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4044</v>
       </c>
       <c r="T48" s="61">
-        <f>A48+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.770787037036</v>
       </c>
     </row>
@@ -26924,11 +26384,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4044*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S49" s="10" t="str">
-        <f>MID(B49,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4044</v>
       </c>
       <c r="T49" s="61">
-        <f>A49+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.771481481483</v>
       </c>
     </row>
@@ -26990,11 +26450,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4013*20160707*" /stext=" 22:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S50" s="10" t="str">
-        <f>MID(B50,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4013</v>
       </c>
       <c r="T50" s="61">
-        <f>A50+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.944618055553</v>
       </c>
     </row>
@@ -27056,11 +26516,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4017*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S51" s="10" t="str">
-        <f>MID(B51,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
       <c r="T51" s="61">
-        <f>A51+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.770891203705</v>
       </c>
     </row>
@@ -27122,11 +26582,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4017*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S52" s="10" t="str">
-        <f>MID(B52,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
       <c r="T52" s="61">
-        <f>A52+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.771585648145</v>
       </c>
     </row>
@@ -27188,11 +26648,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4011*20160707*" /stext=" 15:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S53" s="10" t="str">
-        <f>MID(B53,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4011</v>
       </c>
       <c r="T53" s="61">
-        <f>A53+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.689502314817</v>
       </c>
     </row>
@@ -27254,11 +26714,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S54" s="10" t="str">
-        <f>MID(B54,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4040</v>
       </c>
       <c r="T54" s="61">
-        <f>A54+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.770810185182</v>
       </c>
     </row>
@@ -27320,11 +26780,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S55" s="10" t="str">
-        <f>MID(B55,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4040</v>
       </c>
       <c r="T55" s="61">
-        <f>A55+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.771493055552</v>
       </c>
     </row>
@@ -27386,11 +26846,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4026*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S56" s="10" t="str">
-        <f>MID(B56,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4026</v>
       </c>
       <c r="T56" s="61">
-        <f>A56+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.596203703702</v>
       </c>
     </row>
@@ -27452,11 +26912,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S57" s="10" t="str">
-        <f>MID(B57,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4037</v>
       </c>
       <c r="T57" s="61">
-        <f>A57+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.770289351851</v>
       </c>
     </row>
@@ -27518,11 +26978,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4027*20160707*" /stext=" 15:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S58" s="10" t="str">
-        <f>MID(B58,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4027</v>
       </c>
       <c r="T58" s="61">
-        <f>A58+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.654918981483</v>
       </c>
     </row>
@@ -27584,11 +27044,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4007*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S59" s="10" t="str">
-        <f>MID(B59,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4007</v>
       </c>
       <c r="T59" s="61">
-        <f>A59+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.770613425928</v>
       </c>
     </row>
@@ -27650,11 +27110,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 20:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S60" s="10" t="str">
-        <f>MID(B60,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4012</v>
       </c>
       <c r="T60" s="61">
-        <f>A60+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.855636574073</v>
       </c>
     </row>
@@ -27714,11 +27174,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4028*20160707*" /stext=" 10:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S61" s="10" t="str">
-        <f>MID(B61,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4028</v>
       </c>
       <c r="T61" s="61">
-        <f>A61+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.471574074072</v>
       </c>
     </row>
@@ -27778,11 +27238,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4017*20160707*" /stext=" 11:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S62" s="10" t="str">
-        <f>MID(B62,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
       <c r="T62" s="61">
-        <f>A62+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.501944444448</v>
       </c>
     </row>
@@ -27842,11 +27302,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4032*20160707*" /stext=" 12:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S63" s="10" t="str">
-        <f>MID(B63,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4032</v>
       </c>
       <c r="T63" s="61">
-        <f>A63+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.543634259258</v>
       </c>
     </row>
@@ -27906,11 +27366,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S64" s="10" t="str">
-        <f>MID(B64,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4012</v>
       </c>
       <c r="T64" s="61">
-        <f>A64+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.585405092592</v>
       </c>
     </row>
@@ -27970,11 +27430,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4008*20160707*" /stext=" 15:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S65" s="10" t="str">
-        <f>MID(B65,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4008</v>
       </c>
       <c r="T65" s="61">
-        <f>A65+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.669016203705</v>
       </c>
     </row>
@@ -28034,11 +27494,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4032*20160707*" /stext=" 15:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S66" s="10" t="str">
-        <f>MID(B66,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4032</v>
       </c>
       <c r="T66" s="61">
-        <f>A66+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.689675925925</v>
       </c>
     </row>
@@ -28098,11 +27558,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S67" s="10" t="str">
-        <f>MID(B67,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4043</v>
       </c>
       <c r="T67" s="61">
-        <f>A67+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.751851851855</v>
       </c>
     </row>
@@ -28162,11 +27622,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4032*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S68" s="10" t="str">
-        <f>MID(B68,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4032</v>
       </c>
       <c r="T68" s="61">
-        <f>A68+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.765879629631</v>
       </c>
     </row>
@@ -28226,11 +27686,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4017*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S69" s="10" t="str">
-        <f>MID(B69,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
       <c r="T69" s="61">
-        <f>A69+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.794409722221</v>
       </c>
     </row>
@@ -28290,11 +27750,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 18:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S70" s="10" t="str">
-        <f>MID(B70,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4012</v>
       </c>
       <c r="T70" s="61">
-        <f>A70+6/24</f>
+        <f t="shared" si="3"/>
         <v>42558.804328703707</v>
       </c>
     </row>
@@ -28354,11 +27814,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 19:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S71" s="10" t="str">
-        <f>MID(B71,13,4)</f>
+        <f t="shared" ref="S71:S102" si="4">MID(B71,13,4)</f>
         <v>4043</v>
       </c>
       <c r="T71" s="61">
-        <f>A71+6/24</f>
+        <f t="shared" ref="T71:T102" si="5">A71+6/24</f>
         <v>42558.82471064815</v>
       </c>
     </row>
@@ -28418,11 +27878,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4032*20160707*" /stext=" 19:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S72" s="10" t="str">
-        <f>MID(B72,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4032</v>
       </c>
       <c r="T72" s="61">
-        <f>A72+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.835509259261</v>
       </c>
     </row>
@@ -28482,11 +27942,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4012*20160707*" /stext=" 20:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S73" s="10" t="str">
-        <f>MID(B73,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4012</v>
       </c>
       <c r="T73" s="61">
-        <f>A73+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.881620370368</v>
       </c>
     </row>
@@ -28546,11 +28006,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4013*20160707*" /stext=" 22:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S74" s="10" t="str">
-        <f>MID(B74,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4013</v>
       </c>
       <c r="T74" s="61">
-        <f>A74+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.962800925925</v>
       </c>
     </row>
@@ -28610,11 +28070,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160707*" /stext=" 22:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S75" s="10" t="str">
-        <f>MID(B75,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4043</v>
       </c>
       <c r="T75" s="61">
-        <f>A75+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.971215277779</v>
       </c>
     </row>
@@ -28674,11 +28134,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4017*20160707*" /stext=" 23:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S76" s="10" t="str">
-        <f>MID(B76,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4017</v>
       </c>
       <c r="T76" s="61">
-        <f>A76+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.012453703705</v>
       </c>
     </row>
@@ -28738,11 +28198,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4043*20160708*" /stext=" 00:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S77" s="10" t="str">
-        <f>MID(B77,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4043</v>
       </c>
       <c r="T77" s="61">
-        <f>A77+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.044074074074</v>
       </c>
     </row>
@@ -28802,11 +28262,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4032*20160708*" /stext=" 04:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S78" s="10" t="str">
-        <f>MID(B78,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4032</v>
       </c>
       <c r="T78" s="61">
-        <f>A78+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.210520833331</v>
       </c>
     </row>
@@ -28866,11 +28326,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4037*20160708*" /stext=" 06:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S79" s="10" t="str">
-        <f>MID(B79,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4037</v>
       </c>
       <c r="T79" s="61">
-        <f>A79+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.314282407409</v>
       </c>
     </row>
@@ -28930,11 +28390,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4026*20160707*" /stext=" 11:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S80" s="10" t="str">
-        <f>MID(B80,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4026</v>
       </c>
       <c r="T80" s="61">
-        <f>A80+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.475590277776</v>
       </c>
     </row>
@@ -28994,11 +28454,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 11:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S81" s="10" t="str">
-        <f>MID(B81,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4025</v>
       </c>
       <c r="T81" s="61">
-        <f>A81+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.502662037034</v>
       </c>
     </row>
@@ -29058,11 +28518,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S82" s="10" t="str">
-        <f>MID(B82,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T82" s="61">
-        <f>A82+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.565520833334</v>
       </c>
     </row>
@@ -29122,11 +28582,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S83" s="10" t="str">
-        <f>MID(B83,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4025</v>
       </c>
       <c r="T83" s="61">
-        <f>A83+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.586643518516</v>
       </c>
     </row>
@@ -29186,11 +28646,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160707*" /stext=" 22:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S84" s="10" t="str">
-        <f>MID(B84,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T84" s="61">
-        <f>A84+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.940138888887</v>
       </c>
     </row>
@@ -29250,11 +28710,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 00:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S85" s="10" t="str">
-        <f>MID(B85,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T85" s="61">
-        <f>A85+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.023587962962</v>
       </c>
     </row>
@@ -29314,11 +28774,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160708*" /stext=" 00:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S86" s="10" t="str">
-        <f>MID(B86,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4025</v>
       </c>
       <c r="T86" s="61">
-        <f>A86+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.046099537038</v>
       </c>
     </row>
@@ -29378,11 +28838,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S87" s="10" t="str">
-        <f>MID(B87,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T87" s="61">
-        <f>A87+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.065949074073</v>
       </c>
     </row>
@@ -29442,11 +28902,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 01:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S88" s="10" t="str">
-        <f>MID(B88,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T88" s="61">
-        <f>A88+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.066840277781</v>
       </c>
     </row>
@@ -29506,11 +28966,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4040*20160708*" /stext=" 03:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S89" s="10" t="str">
-        <f>MID(B89,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4040</v>
       </c>
       <c r="T89" s="61">
-        <f>A89+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.148958333331</v>
       </c>
     </row>
@@ -29570,11 +29030,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4025*20160707*" /stext=" 10:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S90" s="10" t="str">
-        <f>MID(B90,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4025</v>
       </c>
       <c r="T90" s="61">
-        <f>A90+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.459328703706</v>
       </c>
     </row>
@@ -29634,11 +29094,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4031*20160707*" /stext=" 11:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S91" s="10" t="str">
-        <f>MID(B91,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4031</v>
       </c>
       <c r="T91" s="61">
-        <f>A91+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.503831018519</v>
       </c>
     </row>
@@ -29698,11 +29158,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4007*20160707*" /stext=" 12:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S92" s="10" t="str">
-        <f>MID(B92,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4007</v>
       </c>
       <c r="T92" s="61">
-        <f>A92+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.555717592593</v>
       </c>
     </row>
@@ -29762,11 +29222,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4038*20160707*" /stext=" 13:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S93" s="10" t="str">
-        <f>MID(B93,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4038</v>
       </c>
       <c r="T93" s="61">
-        <f>A93+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.597858796296</v>
       </c>
     </row>
@@ -29826,11 +29286,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4031*20160707*" /stext=" 14:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S94" s="10" t="str">
-        <f>MID(B94,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4031</v>
       </c>
       <c r="T94" s="61">
-        <f>A94+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.64980324074</v>
       </c>
     </row>
@@ -29890,11 +29350,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4027*20160707*" /stext=" 15:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S95" s="10" t="str">
-        <f>MID(B95,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4027</v>
       </c>
       <c r="T95" s="61">
-        <f>A95+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.662592592591</v>
       </c>
     </row>
@@ -29954,11 +29414,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4007*20160707*" /stext=" 16:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S96" s="10" t="str">
-        <f>MID(B96,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4007</v>
       </c>
       <c r="T96" s="61">
-        <f>A96+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.701273148145</v>
       </c>
     </row>
@@ -30018,11 +29478,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4027*20160707*" /stext=" 16:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S97" s="10" t="str">
-        <f>MID(B97,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4027</v>
       </c>
       <c r="T97" s="61">
-        <f>A97+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.733287037037</v>
       </c>
     </row>
@@ -30082,11 +29542,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4011*20160707*" /stext=" 17:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S98" s="10" t="str">
-        <f>MID(B98,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4011</v>
       </c>
       <c r="T98" s="61">
-        <f>A98+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.764351851853</v>
       </c>
     </row>
@@ -30146,11 +29606,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4038*20160707*" /stext=" 20:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S99" s="10" t="str">
-        <f>MID(B99,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4038</v>
       </c>
       <c r="T99" s="61">
-        <f>A99+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.890243055554</v>
       </c>
     </row>
@@ -30210,11 +29670,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4011*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S100" s="10" t="str">
-        <f>MID(B100,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4011</v>
       </c>
       <c r="T100" s="61">
-        <f>A100+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.911099537036</v>
       </c>
     </row>
@@ -30274,11 +29734,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4014*20160707*" /stext=" 21:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S101" s="10" t="str">
-        <f>MID(B101,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4014</v>
       </c>
       <c r="T101" s="61">
-        <f>A101+6/24</f>
+        <f t="shared" si="5"/>
         <v>42558.920474537037</v>
       </c>
     </row>
@@ -30338,11 +29798,11 @@
         <v>"C:\Program Files (x86)\AstroGrep\AstroGrep.exe" /spath="C:\Users\stu\Documents\Analysis\2016-02-23 RTDC Observations" /stypes="*4018*20160708*" /stext=" 04:.+((prompt.+disp)|(slice.+state.+chan)|(ment ac)|(system.+state.+chan)|(\|lc)|(penalty)|(\[timeout))" /e /r /s</v>
       </c>
       <c r="S102" s="10" t="str">
-        <f>MID(B102,13,4)</f>
+        <f t="shared" si="4"/>
         <v>4018</v>
       </c>
       <c r="T102" s="61">
-        <f>A102+6/24</f>
+        <f t="shared" si="5"/>
         <v>42559.212129629632</v>
       </c>
     </row>
@@ -30662,17 +30122,17 @@
     <mergeCell ref="A5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:N6 P6 M7:M1048576">
-    <cfRule type="cellIs" dxfId="76" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L103:N120 A7:N102">
-    <cfRule type="expression" dxfId="75" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$M7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="74" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>